<commit_message>
v2.2.2 fixed folders paths, plots, gtm_lr
</commit_message>
<xml_diff>
--- a/GridSearch.xlsx
+++ b/GridSearch.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfrazzetto00\PycharmProjects\GTMBasedGraphAggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43851D58-266C-4365-9AA0-48204B7B619E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAABE3F8-920B-4691-9D40-CF9DB641D765}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="1" xr2:uid="{180FEC4F-2D3A-45FB-8208-FE0F44B3C909}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="2" xr2:uid="{180FEC4F-2D3A-45FB-8208-FE0F44B3C909}"/>
   </bookViews>
   <sheets>
     <sheet name="v1_MUTAG" sheetId="1" r:id="rId1"/>
     <sheet name="v2_MUTAG" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="v2_2_MUTAG" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="46">
   <si>
     <t>GTM Grid</t>
   </si>
@@ -138,13 +138,49 @@
   </si>
   <si>
     <t>Per GPU tieni 25Gb</t>
+  </si>
+  <si>
+    <t>ü</t>
+  </si>
+  <si>
+    <t>collate_fn</t>
+  </si>
+  <si>
+    <t>flush output HPC</t>
+  </si>
+  <si>
+    <t>da batch a dataset per PCA e incremental Learning (e labels)</t>
+  </si>
+  <si>
+    <t>ancora for grid search…</t>
+  </si>
+  <si>
+    <t>With validation set; no weight decay; no dropout</t>
+  </si>
+  <si>
+    <t>W/o validation set; no weight decay; no dropout</t>
+  </si>
+  <si>
+    <t>Learning RATE forse ancora troppo alto</t>
+  </si>
+  <si>
+    <t>Scrivi log su home e non Storage</t>
+  </si>
+  <si>
+    <t>ppn per più cores</t>
+  </si>
+  <si>
+    <t>GTM Calssifier / Discarded</t>
+  </si>
+  <si>
+    <t>TODO: Train su NCI () + Incremental Learning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +194,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -303,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -320,6 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -335,7 +378,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1006,6 +1058,536 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>132906</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>60761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1420942</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2277C85A-875C-4227-A2D7-FA8E8ED09A30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2316467" y="1637778"/>
+          <a:ext cx="3269416" cy="2217456"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>694426</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>155277</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1333319</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>43133</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{927CC360-578D-48E6-9D6E-B64827C30135}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2136654" y="4010207"/>
+          <a:ext cx="3361606" cy="2165768"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>177380</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>17254</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1074527</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>90578</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12B45EB6-DC2B-49FF-A930-548FCA8B3EF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2360941" y="6325320"/>
+          <a:ext cx="2878527" cy="2000789"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>120769</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>121138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1503872</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>15815</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{230D8680-A86E-426A-B2E0-8D9006B99074}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10248181" y="1829168"/>
+          <a:ext cx="3367177" cy="2361831"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>293298</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1362974</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>50034</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA6ECB44-294E-49DD-A225-1E048924E230}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10420710" y="4364967"/>
+          <a:ext cx="3053750" cy="2137625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>293298</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>69011</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1242204</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>5929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09B1D26C-BCA4-4C59-9789-66C5F70C29BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10420710" y="6711351"/>
+          <a:ext cx="2932980" cy="2199735"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1388315</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>148266</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>256097</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>23104</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53FCE8BB-9FFA-42B3-8662-64E00CC8540F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13478774" y="1550058"/>
+          <a:ext cx="3450565" cy="2503199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1320922</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>107831</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>231175</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>13480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C9F964F-0B0C-42F5-93AE-21E89CC4F554}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13411381" y="4137984"/>
+          <a:ext cx="3493036" cy="2534010"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1372056</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>107830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>689036</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>33968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B2646A3-E8AB-4A80-A1E8-9C7E511799B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5536997" y="1684847"/>
+          <a:ext cx="3279739" cy="2379274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1388813</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>40436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>742952</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>168754</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{359791F3-3AC1-4B27-8A18-60A27625BA3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5553754" y="4245814"/>
+          <a:ext cx="3316898" cy="2406231"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1381,18 +1963,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="5">
@@ -1418,7 +2000,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
+      <c r="B9" s="18"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -1434,8 +2016,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-      <c r="C10" s="18">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19">
         <v>12</v>
       </c>
       <c r="D10" s="8"/>
@@ -1447,8 +2029,8 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -1458,8 +2040,8 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1469,8 +2051,8 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -1480,8 +2062,8 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -1491,8 +2073,8 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1502,8 +2084,8 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -1513,8 +2095,8 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -1524,8 +2106,8 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -1535,8 +2117,8 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="19">
+      <c r="B19" s="18"/>
+      <c r="C19" s="20">
         <v>5</v>
       </c>
       <c r="D19" s="10"/>
@@ -1548,8 +2130,8 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -1559,8 +2141,8 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1570,8 +2152,8 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1581,8 +2163,8 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -1592,8 +2174,8 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -1603,8 +2185,8 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -1614,8 +2196,8 @@
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -1625,8 +2207,8 @@
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -1636,8 +2218,8 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
-      <c r="C28" s="20"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -1647,8 +2229,8 @@
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="17"/>
-      <c r="C29" s="18">
+      <c r="B29" s="18"/>
+      <c r="C29" s="19">
         <v>15</v>
       </c>
       <c r="D29" s="8"/>
@@ -1660,8 +2242,8 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -1671,8 +2253,8 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -1682,8 +2264,8 @@
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -1693,8 +2275,8 @@
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -1704,8 +2286,8 @@
       <c r="J33" s="10"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -1715,8 +2297,8 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -1726,8 +2308,8 @@
       <c r="J35" s="10"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -1737,8 +2319,8 @@
       <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -1748,8 +2330,8 @@
       <c r="J37" s="10"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -1759,10 +2341,10 @@
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="17"/>
+      <c r="B39" s="18"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="17"/>
+      <c r="B40" s="18"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
@@ -1840,8 +2422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D25272C-5D7D-4C44-80F8-537FD37B5CC8}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView topLeftCell="A52" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1909,18 +2491,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="5">
@@ -1946,7 +2528,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
+      <c r="B9" s="18"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -1956,8 +2538,8 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-      <c r="C10" s="18">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19">
         <v>12</v>
       </c>
       <c r="D10" s="8"/>
@@ -1969,8 +2551,8 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -1980,8 +2562,8 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1991,8 +2573,8 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -2002,8 +2584,8 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -2013,8 +2595,8 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -2024,8 +2606,8 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -2035,8 +2617,8 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -2046,8 +2628,8 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -2057,8 +2639,8 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="19">
+      <c r="B19" s="18"/>
+      <c r="C19" s="20">
         <v>5</v>
       </c>
       <c r="D19" s="10"/>
@@ -2070,8 +2652,8 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -2081,8 +2663,8 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -2092,8 +2674,8 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -2103,8 +2685,8 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -2114,8 +2696,8 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -2125,8 +2707,8 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -2136,8 +2718,8 @@
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -2147,8 +2729,8 @@
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -2158,8 +2740,8 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="17"/>
-      <c r="C28" s="20"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -2169,8 +2751,8 @@
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="17"/>
-      <c r="C29" s="18">
+      <c r="B29" s="18"/>
+      <c r="C29" s="19">
         <v>15</v>
       </c>
       <c r="D29" s="8"/>
@@ -2182,8 +2764,8 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -2193,8 +2775,8 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -2204,8 +2786,8 @@
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -2215,8 +2797,8 @@
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="17"/>
-      <c r="C33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -2226,8 +2808,8 @@
       <c r="J33" s="10"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -2237,8 +2819,8 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -2248,8 +2830,8 @@
       <c r="J35" s="10"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -2259,8 +2841,8 @@
       <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -2270,8 +2852,8 @@
       <c r="J37" s="10"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -2281,10 +2863,10 @@
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="17"/>
+      <c r="B39" s="18"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="17"/>
+      <c r="B40" s="18"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
@@ -2306,12 +2888,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>20</v>
       </c>
@@ -2319,52 +2901,61 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="C55" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="21">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C59" s="16">
         <v>44376</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="C60" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="C62" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>31</v>
       </c>
@@ -2394,6 +2985,702 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813A309A-E32D-452A-82E0-C9D75759D379}">
+  <dimension ref="A1:J82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="109" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="28.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="G3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6">
+        <v>15.2</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="H8" s="6">
+        <v>15.2</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="18"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19">
+        <v>12</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="18"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="18"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="18"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="18"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="18"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="10"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="18"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="18"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="18"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="10"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="18"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="18"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="18"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="10"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="18"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="10"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="18"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="10"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="18"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="10"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="18"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="10"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="18"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="10"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="18"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="10"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="18"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="10"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="18"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="18"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="18"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="10"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="18"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="10"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="18"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="10"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="18"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="10"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="18"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="10"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="18"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="10"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="18"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="10"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="18"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="10"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="18"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="18"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="18"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="16">
+        <v>44376</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C69" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C77" s="16">
+        <v>44384</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>37</v>
+      </c>
+      <c r="F78" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>44</v>
+      </c>
+      <c r="F79" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>35</v>
+      </c>
+      <c r="F80" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="B8:B49"/>
+    <mergeCell ref="C10:C18"/>
+    <mergeCell ref="C19:C27"/>
+    <mergeCell ref="C28:C37"/>
+    <mergeCell ref="C38:C47"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5B125D-C5AF-475F-AEEA-8FE09BD19360}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
v 2.3 Incremental Learning
</commit_message>
<xml_diff>
--- a/GridSearch.xlsx
+++ b/GridSearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfrazzetto00\PycharmProjects\GTMBasedGraphAggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02439D38-629F-4B6D-A6FB-2A0C6902913F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62678B7-5A35-48C1-BA15-AEBBC8166B4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="4" xr2:uid="{180FEC4F-2D3A-45FB-8208-FE0F44B3C909}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="2" xr2:uid="{180FEC4F-2D3A-45FB-8208-FE0F44B3C909}"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="6" r:id="rId1"/>
@@ -2614,7 +2614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D25272C-5D7D-4C44-80F8-537FD37B5CC8}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
@@ -3180,7 +3180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813A309A-E32D-452A-82E0-C9D75759D379}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="109" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="109" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
@@ -3876,7 +3876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2F13C0-FE8C-4BB7-8E31-E651CB36AFDB}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="83" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v 2.3.1 fixed Incremental Learning, minor bugs on initialization and memory efficiency
</commit_message>
<xml_diff>
--- a/GridSearch.xlsx
+++ b/GridSearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfrazzetto00\PycharmProjects\GTMBasedGraphAggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62678B7-5A35-48C1-BA15-AEBBC8166B4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9068C6-159C-4BA7-9E75-5C910F6C2CD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="2" xr2:uid="{180FEC4F-2D3A-45FB-8208-FE0F44B3C909}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="5" xr2:uid="{180FEC4F-2D3A-45FB-8208-FE0F44B3C909}"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="v2_MUTAG" sheetId="3" r:id="rId3"/>
     <sheet name="v2_2_MUTAG" sheetId="4" r:id="rId4"/>
     <sheet name="v2_2_NCI" sheetId="5" r:id="rId5"/>
+    <sheet name="v2_3_MUTAG" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="84">
   <si>
     <t>GTM Grid</t>
   </si>
@@ -190,13 +191,112 @@
   </si>
   <si>
     <t>Lanciato test NCI</t>
+  </si>
+  <si>
+    <t>TEST NAME</t>
+  </si>
+  <si>
+    <t>lr_test_2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataset_name: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_fold: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">learning_rate_conv: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">learning_rate_gtm: </t>
+  </si>
+  <si>
+    <t>0.0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">learning_rate_read_out: </t>
+  </si>
+  <si>
+    <t>0.0005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">learning_rate_fine_tuning: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">drop_prob: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight_decay: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_size: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_hidden: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtm_grid_dims: </t>
+  </si>
+  <si>
+    <t>(15, 20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtm_lr: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtm_rbf: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtm_lear: </t>
+  </si>
+  <si>
+    <t>incremental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_epoch: </t>
+  </si>
+  <si>
+    <t>0.1 to  0.0001</t>
+  </si>
+  <si>
+    <t>gtm_lr</t>
+  </si>
+  <si>
+    <t>incremental || standard (batched)</t>
+  </si>
+  <si>
+    <t>batched learning</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>avg epoch time:</t>
+  </si>
+  <si>
+    <t>avg epoch time</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>batched</t>
+  </si>
+  <si>
+    <t>0.19</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +316,14 @@
       <color theme="1"/>
       <name val="Wingdings"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -244,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -357,11 +465,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -379,6 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -394,7 +515,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -404,9 +524,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1590,6 +1713,926 @@
         <a:xfrm>
           <a:off x="5553754" y="4245814"/>
           <a:ext cx="3316898" cy="2406231"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>362309</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>86264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>69011</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>17253</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F124E17-224A-4A13-945B-85E7F12462BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1069675" y="3347049"/>
+          <a:ext cx="4054415" cy="2838091"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>241540</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>60386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>598096</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>34505</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09122FF8-7058-4052-A07E-884F96D3184F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6202393" y="3329797"/>
+          <a:ext cx="4083167" cy="3062376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>198407</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>43130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>405442</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>86263</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD21230E-CEE8-4298-9B5F-2C4E5508F3AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10506973" y="3312541"/>
+          <a:ext cx="3933646" cy="2950235"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>301925</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>14663</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>362310</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>129394</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A15A5C8-3063-49B5-905A-0434E05D815B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1915065" y="6372331"/>
+          <a:ext cx="3786996" cy="2650897"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>517584</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>159588</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>310550</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>81950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A58191E5-3B42-479F-92A8-52490607CBE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6478437" y="6517256"/>
+          <a:ext cx="3519577" cy="2639683"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>23969</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>12150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>47504</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>4374</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{745E1091-8D18-4217-A0F6-07CBA573BB6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10934562" y="6779633"/>
+          <a:ext cx="3121755" cy="2361451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>109350</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>145809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>267299</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>148734</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE0995CE-DA28-4C63-8498-496989062D3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1725284" y="12769534"/>
+          <a:ext cx="3875812" cy="2736649"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>449544</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>32435</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>328047</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>97199</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A22DA4-BA95-46E5-9718-D0E1F9C281E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6402985" y="12838410"/>
+          <a:ext cx="2976723" cy="2251741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>72901</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>52211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>182249</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>109349</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B7EE381-BA3E-454B-A405-70F93FA2C7A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9744205" y="13040434"/>
+          <a:ext cx="3207568" cy="2426364"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>121501</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>85161</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>97200</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>133282</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B32B85D0-B346-4D2F-8C7C-8E2A8FAE003B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6074942" y="9780765"/>
+          <a:ext cx="3693562" cy="2793994"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>315897</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>176071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>109350</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>91729</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A98D74C1-279A-4E0F-B879-50E9DE9FA06F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1931831" y="9871675"/>
+          <a:ext cx="3511316" cy="2479284"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>583194</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>372566</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>101574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A01408C6-746C-4C66-AB4B-3401D6C3C4DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10254498" y="9890003"/>
+          <a:ext cx="3507236" cy="2653048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>194397</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>16387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>187159</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>157948</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E22023D-CE99-45A8-AEBF-665CFA252282}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1810331" y="16673873"/>
+          <a:ext cx="4330269" cy="3057533"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>583195</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>41617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>510296</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>65127</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{206B950D-B732-46BA-86DE-B10D3D82B8C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6536636" y="16699103"/>
+          <a:ext cx="3644964" cy="2757232"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>593066</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>107830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>167699</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>111066</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{167335DC-6C8A-4959-BAB5-EBA59DAA4EE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10890850" y="17845896"/>
+          <a:ext cx="2674749" cy="2078967"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1960,7 +3003,7 @@
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C19" s="15" t="s">
@@ -1983,7 +3026,7 @@
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C24" t="s">
@@ -1996,7 +3039,7 @@
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C26" t="s">
@@ -2024,7 +3067,7 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C33" t="s">
@@ -2155,18 +3198,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="5">
@@ -2192,7 +3235,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
+      <c r="B9" s="19"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -2208,8 +3251,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20">
         <v>12</v>
       </c>
       <c r="D10" s="8"/>
@@ -2221,8 +3264,8 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -2232,8 +3275,8 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -2243,8 +3286,8 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -2254,8 +3297,8 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -2265,8 +3308,8 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -2276,8 +3319,8 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -2287,8 +3330,8 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -2298,8 +3341,8 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -2309,8 +3352,8 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="C19" s="20">
+      <c r="B19" s="19"/>
+      <c r="C19" s="21">
         <v>5</v>
       </c>
       <c r="D19" s="10"/>
@@ -2322,8 +3365,8 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -2333,8 +3376,8 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -2344,8 +3387,8 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -2355,8 +3398,8 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -2366,8 +3409,8 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -2377,8 +3420,8 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -2388,8 +3431,8 @@
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -2399,8 +3442,8 @@
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -2410,8 +3453,8 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="18"/>
-      <c r="C28" s="21"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -2421,8 +3464,8 @@
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="18"/>
-      <c r="C29" s="19">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20">
         <v>15</v>
       </c>
       <c r="D29" s="8"/>
@@ -2434,8 +3477,8 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -2445,8 +3488,8 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -2456,8 +3499,8 @@
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -2467,8 +3510,8 @@
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -2478,8 +3521,8 @@
       <c r="J33" s="10"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -2489,8 +3532,8 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -2500,8 +3543,8 @@
       <c r="J35" s="10"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -2511,8 +3554,8 @@
       <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -2522,8 +3565,8 @@
       <c r="J37" s="10"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -2533,10 +3576,10 @@
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="18"/>
+      <c r="B39" s="19"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="18"/>
+      <c r="B40" s="19"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
@@ -2614,7 +3657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D25272C-5D7D-4C44-80F8-537FD37B5CC8}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="58" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
@@ -2683,18 +3726,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="5">
@@ -2720,7 +3763,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
+      <c r="B9" s="19"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -2730,8 +3773,8 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20">
         <v>12</v>
       </c>
       <c r="D10" s="8"/>
@@ -2743,8 +3786,8 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -2754,8 +3797,8 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -2765,8 +3808,8 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -2776,8 +3819,8 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -2787,8 +3830,8 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -2798,8 +3841,8 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -2809,8 +3852,8 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -2820,8 +3863,8 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -2831,8 +3874,8 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="C19" s="20">
+      <c r="B19" s="19"/>
+      <c r="C19" s="21">
         <v>5</v>
       </c>
       <c r="D19" s="10"/>
@@ -2844,8 +3887,8 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -2855,8 +3898,8 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -2866,8 +3909,8 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -2877,8 +3920,8 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -2888,8 +3931,8 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -2899,8 +3942,8 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -2910,8 +3953,8 @@
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -2921,8 +3964,8 @@
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -2932,8 +3975,8 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="18"/>
-      <c r="C28" s="21"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -2943,8 +3986,8 @@
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="18"/>
-      <c r="C29" s="19">
+      <c r="B29" s="19"/>
+      <c r="C29" s="20">
         <v>15</v>
       </c>
       <c r="D29" s="8"/>
@@ -2956,8 +3999,8 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -2967,8 +4010,8 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -2978,8 +4021,8 @@
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -2989,8 +4032,8 @@
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -3000,8 +4043,8 @@
       <c r="J33" s="10"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -3011,8 +4054,8 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -3022,8 +4065,8 @@
       <c r="J35" s="10"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -3033,8 +4076,8 @@
       <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -3044,8 +4087,8 @@
       <c r="J37" s="10"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -3055,10 +4098,10 @@
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="18"/>
+      <c r="B39" s="19"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="18"/>
+      <c r="B40" s="19"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
@@ -3104,7 +4147,7 @@
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C55" s="15" t="s">
@@ -3127,7 +4170,7 @@
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="22" t="s">
+      <c r="B60" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C60" t="s">
@@ -3140,7 +4183,7 @@
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C62" t="s">
@@ -3249,18 +4292,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="5"/>
@@ -3275,7 +4318,7 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
+      <c r="B9" s="19"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
         <v>39</v>
@@ -3289,8 +4332,8 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20">
         <v>12</v>
       </c>
       <c r="D10" s="8"/>
@@ -3302,8 +4345,8 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -3313,8 +4356,8 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -3324,8 +4367,8 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -3335,8 +4378,8 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -3346,8 +4389,8 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -3357,8 +4400,8 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -3368,8 +4411,8 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -3379,8 +4422,8 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -3390,7 +4433,7 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="23"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -3401,7 +4444,7 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="18"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="24"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -3412,7 +4455,7 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="18"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="24"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -3423,7 +4466,7 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="18"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="24"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -3434,7 +4477,7 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="18"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="24"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -3445,7 +4488,7 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="18"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="24"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -3456,7 +4499,7 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="24"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -3467,7 +4510,7 @@
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="18"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="24"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -3478,7 +4521,7 @@
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="18"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="25"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -3489,7 +4532,7 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="18"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="23"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -3500,7 +4543,7 @@
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="18"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="24"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -3511,7 +4554,7 @@
       <c r="J29" s="10"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="18"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="24"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
@@ -3522,7 +4565,7 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="18"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="24"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -3533,7 +4576,7 @@
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="18"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="24"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -3544,7 +4587,7 @@
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="18"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="24"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
@@ -3555,7 +4598,7 @@
       <c r="J33" s="10"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="18"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="24"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -3566,7 +4609,7 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="18"/>
+      <c r="B35" s="19"/>
       <c r="C35" s="24"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -3577,7 +4620,7 @@
       <c r="J35" s="10"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="18"/>
+      <c r="B36" s="19"/>
       <c r="C36" s="24"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
@@ -3588,7 +4631,7 @@
       <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="18"/>
+      <c r="B37" s="19"/>
       <c r="C37" s="25"/>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
@@ -3599,7 +4642,7 @@
       <c r="J37" s="11"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="18"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="23"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
@@ -3610,7 +4653,7 @@
       <c r="J38" s="8"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="18"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="24"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -3621,7 +4664,7 @@
       <c r="J39" s="10"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="18"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="24"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
@@ -3632,7 +4675,7 @@
       <c r="J40" s="10"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="18"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="24"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -3643,7 +4686,7 @@
       <c r="J41" s="10"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="18"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="24"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -3654,7 +4697,7 @@
       <c r="J42" s="10"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="18"/>
+      <c r="B43" s="19"/>
       <c r="C43" s="24"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -3665,7 +4708,7 @@
       <c r="J43" s="10"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="18"/>
+      <c r="B44" s="19"/>
       <c r="C44" s="24"/>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -3676,7 +4719,7 @@
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="18"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="24"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
@@ -3689,7 +4732,7 @@
       <c r="J45" s="10"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="18"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="24"/>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
@@ -3700,7 +4743,7 @@
       <c r="J46" s="10"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="18"/>
+      <c r="B47" s="19"/>
       <c r="C47" s="25"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
@@ -3711,10 +4754,10 @@
       <c r="J47" s="11"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="18"/>
+      <c r="B48" s="19"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="18"/>
+      <c r="B49" s="19"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
@@ -3760,7 +4803,7 @@
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C64" s="15" t="s">
@@ -3783,7 +4826,7 @@
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="22" t="s">
+      <c r="B69" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C69" t="s">
@@ -3796,7 +4839,7 @@
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="17" t="s">
         <v>34</v>
       </c>
       <c r="C71" t="s">
@@ -3944,17 +4987,17 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="15"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" s="16"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
+      <c r="B23" s="17"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="22"/>
+      <c r="B25" s="17"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" s="16"/>
@@ -3963,4 +5006,251 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BFA4D5-77A8-425A-ACAA-5906E6160E7C}">
+  <dimension ref="A1:F98"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="32" workbookViewId="0">
+      <selection activeCell="P93" sqref="P93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="26">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+    </row>
+    <row r="19" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+    </row>
+    <row r="54" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="27"/>
+    </row>
+    <row r="89" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add PTC, log-likelihood. Fixing inc learning
</commit_message>
<xml_diff>
--- a/GridSearch.xlsx
+++ b/GridSearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfrazzetto00\PycharmProjects\GTMBasedGraphAggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9068C6-159C-4BA7-9E75-5C910F6C2CD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46450359-079A-4A94-8551-80E7FAA110A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="5" xr2:uid="{180FEC4F-2D3A-45FB-8208-FE0F44B3C909}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="6" xr2:uid="{180FEC4F-2D3A-45FB-8208-FE0F44B3C909}"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="v2_2_MUTAG" sheetId="4" r:id="rId4"/>
     <sheet name="v2_2_NCI" sheetId="5" r:id="rId5"/>
     <sheet name="v2_3_MUTAG" sheetId="7" r:id="rId6"/>
+    <sheet name="v2_4_MUTAG" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="93">
   <si>
     <t>GTM Grid</t>
   </si>
@@ -290,6 +291,33 @@
   </si>
   <si>
     <t>0.18</t>
+  </si>
+  <si>
+    <t>NOTE:</t>
+  </si>
+  <si>
+    <t>Con incremental learning ci sono da cambiare tutti gli ipreparametri?</t>
+  </si>
+  <si>
+    <t>Salvare gli output delle conv senza ricalcolarle, shuffle batch</t>
+  </si>
+  <si>
+    <t>Risolvere memory leak su NCI, GTM +s sec ogni iterazione</t>
+  </si>
+  <si>
+    <t>TODO:</t>
+  </si>
+  <si>
+    <t>Incremental learning con batch=1</t>
+  </si>
+  <si>
+    <t>PTC in locale è più significativo</t>
+  </si>
+  <si>
+    <t>No regolarizzare NCI</t>
+  </si>
+  <si>
+    <t>0.1</t>
   </si>
 </sst>
 </file>
@@ -2617,7 +2645,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2633,6 +2661,2220 @@
         <a:xfrm>
           <a:off x="10890850" y="17845896"/>
           <a:ext cx="2674749" cy="2078967"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>107832</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>33080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>504647</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>124006</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70D650AA-B248-4E53-9978-330EC8A7FCF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2345307" y="20979096"/>
+          <a:ext cx="3496934" cy="2544060"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>80871</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>112191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>239608</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>107830</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B03C2695-AB62-4E68-9CE6-B73C52591105}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6038490" y="20680800"/>
+          <a:ext cx="3878877" cy="3014883"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>431323</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>134785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>595562</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>30193</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21CE191A-34D5-4A0D-8448-4FA92ECE0564}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10109082" y="21080801"/>
+          <a:ext cx="3264358" cy="2537245"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251603</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>143773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>378890</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>107829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78CBBCD8-FF75-4B44-8F58-C5321660312B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1869057" y="23506981"/>
+          <a:ext cx="3793512" cy="2659811"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>150026</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>112518</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>455928</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>138025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACA3988B-4D30-4AEA-A706-3EC77C8AE6F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6226022" y="24491518"/>
+          <a:ext cx="3493928" cy="2650937"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>562590</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>29085</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>3116</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C15C3ACE-D78A-4CD0-8470-90CA5DEF994F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9826612" y="24408085"/>
+          <a:ext cx="3900640" cy="2959521"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>544825</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>136208</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381755</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>92624</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3CF2224-15C5-4FF7-9C78-5F4051523EA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5993088" y="27740734"/>
+          <a:ext cx="3650714" cy="2680548"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>317816</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>45401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>210566</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>43133</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AF4BE11-9717-4D01-BCCC-2A567D122DFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1952295" y="27831538"/>
+          <a:ext cx="3706534" cy="2540253"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>136204</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>544822</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>145681</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD67511B-CC63-405C-9062-AAF68FF3F35D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9897675" y="28103951"/>
+          <a:ext cx="3722979" cy="2733609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>362309</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>86264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>69011</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>17253</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{742353BE-AB56-467D-836C-5265EDC9B05F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1975449" y="3355675"/>
+          <a:ext cx="4054415" cy="2838091"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>241540</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>60386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>888</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>34505</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FCCC500-1BED-4E5F-80D1-EF3C25B38559}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6202393" y="3329797"/>
+          <a:ext cx="4083167" cy="3062376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>198407</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>43130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>405442</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>86263</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5C2D897-AFC7-426C-89ED-04D945EB1A7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10506973" y="3312541"/>
+          <a:ext cx="3933646" cy="2950235"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>121501</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>85161</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>97200</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>133282</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12480850-50E0-4CBD-BB11-54095285A7E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6082354" y="9712240"/>
+          <a:ext cx="3702310" cy="2774068"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>315897</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>176071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>109350</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>91729</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{421FD228-A165-4397-94C1-7010C5FFB4C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1929037" y="9803150"/>
+          <a:ext cx="3520064" cy="2460451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>583194</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>372566</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>101574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4328045A-C96F-4F40-8B03-04F086ABC865}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10270658" y="9816860"/>
+          <a:ext cx="3515983" cy="2637740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>194397</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>16387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>187159</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>157948</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3CFD739-1E67-4812-893F-A2D65D51EDCB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1807537" y="16553225"/>
+          <a:ext cx="4340475" cy="3040036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>583195</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>41617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>510296</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>65127</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5907CF2F-F233-4B4C-9728-E1FE4C9ADABC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6544048" y="16578455"/>
+          <a:ext cx="3653712" cy="2740830"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>593066</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>107830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>167699</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>111066</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{482F6113-9B5B-48A7-A49F-83B0C909F2DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10901632" y="17188132"/>
+          <a:ext cx="2680142" cy="1995938"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>251603</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>143773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>378890</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>107829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74C23457-E02F-44B4-B93D-8785D37AB906}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1864743" y="23762898"/>
+          <a:ext cx="3853898" cy="2681376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>150026</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>112518</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>455928</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>138025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E4301C8-C58D-4B85-933F-8FB81A162108}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6110879" y="23731643"/>
+          <a:ext cx="3411411" cy="2561673"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>562590</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>29085</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>3116</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3D5FDB3-EE15-4DA8-901D-8A92978281C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9628952" y="23648210"/>
+          <a:ext cx="3785123" cy="2872506"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>270764</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>109792</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>432103</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>12549</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A0E11CB-5B6F-4914-A4E9-84C9FFAC5F80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10669515" y="7073661"/>
+          <a:ext cx="3298217" cy="2537735"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>141159</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>132631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533269</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>106655</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32835D14-B5B8-4A5F-9D4B-DB7A763BD77B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6775657" y="7284713"/>
+          <a:ext cx="2901612" cy="2232577"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>188213</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152379</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>416423</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>11761</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11DACB9D-44A5-4BFA-86F9-DB0FC70A7883}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1803706" y="6739823"/>
+          <a:ext cx="3992462" cy="2870785"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>170286</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>94106</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>82997</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>33003</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF4CC7A1-33D8-4194-9506-3B8212454B13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1785779" y="13080782"/>
+          <a:ext cx="3676963" cy="2573874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57508</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>62737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>580321</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>6637</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33FA00F3-ECA4-4766-AB00-321C4A72377F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6064630" y="13237626"/>
+          <a:ext cx="3659691" cy="2744769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>298003</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>184291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>292775</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>2767</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ECDA19D-C0DF-4CBF-9C02-54EFD0CD91FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6305125" y="20699475"/>
+          <a:ext cx="3759026" cy="2819270"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>389869</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>47053</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7342</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>17316</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AB835DF-7468-4488-82DF-C80F9E640119}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2005362" y="20750449"/>
+          <a:ext cx="3990649" cy="2793454"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>141159</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>188211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>322746</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>127107</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EFF3D17-5734-4E25-A52A-9AB80DA51217}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1756652" y="28420115"/>
+          <a:ext cx="3945839" cy="2762087"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>94106</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>58816</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>214353</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>54894</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{667516A4-DE01-485A-AE3A-420DC887407E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6101228" y="28478932"/>
+          <a:ext cx="3257125" cy="2442844"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>177756</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>109791</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>104563</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>149002</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF77863B-70B1-45E0-ACBA-7B40646D7D5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6184878" y="35117351"/>
+          <a:ext cx="4318436" cy="3238827"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>156844</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>31369</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>564638</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>149001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{124DF4A8-A9D5-451F-95B0-FAD22E4BE678}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6163966" y="31839314"/>
+          <a:ext cx="4172048" cy="3129036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>31371</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>94107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190551</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>17320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BF68130-B190-4E03-9B97-6E099B671776}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1646864" y="32278478"/>
+          <a:ext cx="3923432" cy="2746402"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>608922</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>144269</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>507435</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>112652</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14D75B44-A038-47DA-B734-08D5BB103DA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10148722" y="12576454"/>
+          <a:ext cx="3552054" cy="2632424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>117634</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>156843</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>283635</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>59602</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D4B7CE6-6E89-43EA-8099-00CAFDD80B3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10508543" y="21526825"/>
+          <a:ext cx="3302878" cy="2647527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>355206</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>70205</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>380576</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>36536</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B2DB08D-5FC0-4EBF-957E-3C3C375F1BD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9895006" y="26710605"/>
+          <a:ext cx="3069988" cy="2275166"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>159752</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>63898</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>387517</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>106071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66E45456-BFCF-4360-A4E1-3B037906F668}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10255852" y="35911446"/>
+          <a:ext cx="3870028" cy="3109344"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>127798</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>102238</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>523129</xdr:colOff>
+      <xdr:row>204</xdr:row>
+      <xdr:rowOff>53083</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4A51203-B617-4CA7-A294-48DE0D049F86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1725283" y="36333182"/>
+          <a:ext cx="4037594" cy="2826316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>132714</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>132712</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>300413</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>5307</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79747A38-8120-4008-BCE0-ACC21B7BBB34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10683483" y="33974804"/>
+          <a:ext cx="3153768" cy="2659588"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3657,7 +5899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D25272C-5D7D-4C44-80F8-537FD37B5CC8}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView zoomScale="58" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="G7" zoomScale="153" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
@@ -4223,7 +6465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813A309A-E32D-452A-82E0-C9D75759D379}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="109" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
@@ -5010,10 +7252,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2BFA4D5-77A8-425A-ACAA-5906E6160E7C}">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:AA128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="32" workbookViewId="0">
-      <selection activeCell="P93" sqref="P93"/>
+    <sheetView zoomScale="31" workbookViewId="0">
+      <selection activeCell="AD102" sqref="AD102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -5021,7 +7263,7 @@
     <col min="1" max="1" width="23.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -5029,7 +7271,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -5037,7 +7279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -5045,7 +7287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -5053,39 +7295,51 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="AA5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="AA6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>60</v>
       </c>
       <c r="B7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="AA7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="AA8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -5093,7 +7347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -5101,7 +7355,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -5109,7 +7363,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -5117,36 +7371,48 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="AA13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>68</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="AA14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>69</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="AA15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
       <c r="B16">
         <v>1</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -5248,6 +7514,346 @@
         <v>83</v>
       </c>
     </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B127" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C127" s="27"/>
+      <c r="D127" s="27"/>
+      <c r="E127" s="27"/>
+      <c r="F127" s="27"/>
+    </row>
+    <row r="128" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEFDB3D-11D2-4AC3-AC6A-E8ACDB327B1B}">
+  <dimension ref="A1:AA170"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="13" workbookViewId="0">
+      <selection activeCell="AU196" sqref="AU196"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="26">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+    </row>
+    <row r="19" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+    </row>
+    <row r="54" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="27"/>
+    </row>
+    <row r="89" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B127" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C127" s="27"/>
+      <c r="D127" s="27"/>
+      <c r="E127" s="27"/>
+      <c r="F127" s="27"/>
+    </row>
+    <row r="128" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B169" s="27">
+        <v>0</v>
+      </c>
+      <c r="C169" s="27"/>
+      <c r="D169" s="27"/>
+      <c r="E169" s="27"/>
+      <c r="F169" s="27"/>
+    </row>
+    <row r="170" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v2.7 added validation loss fr GTM
</commit_message>
<xml_diff>
--- a/GridSearch.xlsx
+++ b/GridSearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfrazzetto00\PycharmProjects\GTMBasedGraphAggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C2FAE4-402C-4095-8649-54005B7AECF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{155D35A3-0DA8-4B74-809A-ADE07CBCDF20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="6" xr2:uid="{180FEC4F-2D3A-45FB-8208-FE0F44B3C909}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="7" xr2:uid="{180FEC4F-2D3A-45FB-8208-FE0F44B3C909}"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="6" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="v2_2_NCI" sheetId="5" r:id="rId5"/>
     <sheet name="v2_3_MUTAG" sheetId="7" r:id="rId6"/>
     <sheet name="v2_4_MUTAG" sheetId="8" r:id="rId7"/>
+    <sheet name="v2_5_MUTAG" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="137">
   <si>
     <t>GTM Grid</t>
   </si>
@@ -321,13 +322,142 @@
   </si>
   <si>
     <t>batch size 12</t>
+  </si>
+  <si>
+    <t>Test Name:</t>
+  </si>
+  <si>
+    <t>test_2_5</t>
+  </si>
+  <si>
+    <t>n_units_list = [30]</t>
+  </si>
+  <si>
+    <t>lr_conv = 0.0005</t>
+  </si>
+  <si>
+    <t>lr_readout = 0.0005</t>
+  </si>
+  <si>
+    <t>lr_fine_tuning = 0.0001</t>
+  </si>
+  <si>
+    <t>drop_prob_list = [0, 0.5]</t>
+  </si>
+  <si>
+    <t>weight_decay_list = [5e-4, 0]</t>
+  </si>
+  <si>
+    <t>batch_size_list = [16, 32]</t>
+  </si>
+  <si>
+    <t>gtm_epoch = 25</t>
+  </si>
+  <si>
+    <t>gtm_grids_dim_list = [(18, 20), (15, 20), (10,15)]</t>
+  </si>
+  <si>
+    <t>gtm_lr_list = [10, 1, 1e-2, 0]</t>
+  </si>
+  <si>
+    <t>gtm_sigma_list = [None, 1]</t>
+  </si>
+  <si>
+    <t>gtm_learning = 'incremental'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtm_rbf_list = [8, 12, 18] </t>
+  </si>
+  <si>
+    <t>Grid Search with 576 points:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEST TEST </t>
+  </si>
+  <si>
+    <t>(18, 20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gtm_sigma: </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Biggest Grid</t>
+  </si>
+  <si>
+    <t>Smallest Sigma</t>
+  </si>
+  <si>
+    <t>drop_prob-0_weight-decay-0.0005_batchSize-32_nHidden-30_grid-18_20_lr-1_lear-incremental_rbf-12_s-None</t>
+  </si>
+  <si>
+    <t>drop_prob-0.5_weight-decay-0_batchSize-32_nHidden-30_grid-15_20_lr-1_lear-incremental_rbf-18_s-None</t>
+  </si>
+  <si>
+    <t>drop_prob-0.5_weight-decay-0_batchSize-16_nHidden-30_grid-15_20_lr-1_lear-incremental_rbf-8_s-None</t>
+  </si>
+  <si>
+    <t>drop_prob-0.5_weight-decay-0.0005_batchSize-32_nHidden-30_grid-18_20_lr-1_lear-incremental_rbf-18_s-None</t>
+  </si>
+  <si>
+    <t>drop_prob-0_weight-decay-0.0005_batchSize-32_nHidden-30_grid-10_15_lr-10_lear-incremental_rbf-18_s-None</t>
+  </si>
+  <si>
+    <t>drop_prob-0_weight-decay-0_batchSize-32_nHidden-30_grid-15_20_lr-0_lear-incremental_rbf-18_s-1</t>
+  </si>
+  <si>
+    <t>drop_prob-0_weight-decay-0_batchSize-32_nHidden-30_grid-10_15_lr-0_lear-incremental_rbf-8_s-None</t>
+  </si>
+  <si>
+    <t>TAKEAWAYS:</t>
+  </si>
+  <si>
+    <t>Dropout and weight decay don't seem to influence performances for this dataset (they are negleted anyway to train GTM)</t>
+  </si>
+  <si>
+    <t>GTM REGULARIZATION</t>
+  </si>
+  <si>
+    <t>NO GTM REGULARIZATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x0.01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x10 </t>
+  </si>
+  <si>
+    <t>There should be at least some regularization for GTM</t>
+  </si>
+  <si>
+    <t>RBF SIGMA VALUE</t>
+  </si>
+  <si>
+    <t>Same for batch_size</t>
+  </si>
+  <si>
+    <t>RBF's sigma should be &lt;1</t>
+  </si>
+  <si>
+    <t>RBFs Lattice dimension</t>
+  </si>
+  <si>
+    <t>Other well performing tests (&gt;94%)</t>
+  </si>
+  <si>
+    <t>It performs well also for smaller latent variable grids</t>
+  </si>
+  <si>
+    <t>RBFs should be less than latent variables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +482,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -383,7 +529,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -507,12 +653,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -531,6 +698,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -555,10 +724,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
+    <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="3" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="4" builtinId="19"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
@@ -4936,6 +5112,1292 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>348934</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>244276</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>8575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A92FCA05-8DCC-470F-908E-0A0B42386BB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5030460" y="3896427"/>
+          <a:ext cx="2376649" cy="1812516"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>368317</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>111198</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>112464</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38771</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CC81F25-AE25-4197-8C4E-C5E06530A26A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7531150" y="3988238"/>
+          <a:ext cx="2225452" cy="1585008"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>174468</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>116618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>261702</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>37906</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C537C27D-D03B-4A78-A3BF-027E8F982E5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9818606" y="3809499"/>
+          <a:ext cx="2568540" cy="1958859"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>426476</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>53861</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>494324</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>144524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9376D4E-8C73-40A0-8360-450E4D183C6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10070614" y="6140815"/>
+          <a:ext cx="2549154" cy="1944074"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>459107</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>77540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>254429</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>144526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F5FBCAF-545E-4B28-8ED4-7A01E37B74E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5140633" y="6164494"/>
+          <a:ext cx="2276629" cy="1736237"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>406021</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>215660</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>508</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2B905A5-8C16-4FF2-9C3F-ACF84193FD29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7568854" y="6290499"/>
+          <a:ext cx="2290944" cy="1631652"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>543584</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>82719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>321761</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>158465</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8CCFD39-42D9-4E80-B4F5-16B5B931865C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5246752" y="8425526"/>
+          <a:ext cx="2283383" cy="1671042"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>496315</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>141803</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>425313</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>28124</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC5D9914-EFE2-4337-8C8F-2C203B110A81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7704689" y="8484610"/>
+          <a:ext cx="2434203" cy="1658871"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>570220</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>167338</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>147170</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>1374</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2756356F-1634-4675-83B2-D43B459D7768}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10147003" y="8486711"/>
+          <a:ext cx="2647369" cy="1938092"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190075</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>146479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>131592</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>147378</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{435EF922-C30C-44FD-B34E-DFA3684E4A34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4854187" y="10571282"/>
+          <a:ext cx="2397852" cy="1755425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>497118</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>94792</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>394769</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>125593</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20ABF27F-27F4-4F2E-B2E5-77F9CFB713A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7617565" y="10695048"/>
+          <a:ext cx="2353987" cy="1609874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190075</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>161875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>584841</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>45031</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B103D1C2-3936-4A50-923B-D8282D3BA8BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10380941" y="10586678"/>
+          <a:ext cx="2237019" cy="1637682"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>215661</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>95848</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>523837</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>79552</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4D0EBE0-8A84-4AB7-90EB-7CB74866920C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4912264" y="14113773"/>
+          <a:ext cx="2177234" cy="1708987"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>191698</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>111372</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>167735</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>8624</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{917575DC-D169-42F4-A7BB-F59B6495EC7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7380379" y="14129297"/>
+          <a:ext cx="2468112" cy="1814233"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>191700</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>166663</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>287546</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>9510</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6D11B5D-339F-4922-AE21-E4C536B3C286}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10495472" y="14184588"/>
+          <a:ext cx="1964905" cy="1542323"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>597213</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>33179</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>570061</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>103516</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B533F2B3-8AC1-46D1-9BBD-D060FB7831D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4678171" y="16987402"/>
+          <a:ext cx="2494417" cy="1729264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66358</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>36831</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>66139</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>66357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F61311A2-5C56-40BB-966D-06C6B8611223}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7299273" y="16825162"/>
+          <a:ext cx="3151743" cy="2020237"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>199071</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>16596</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>530858</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>3982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04FC67CB-9CF4-456B-8D99-74CCDB6D4778}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10583948" y="16804927"/>
+          <a:ext cx="2853352" cy="1978097"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>132714</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>101477</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>398141</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>103516</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0F0C1E0-A4C8-49AE-ACD4-63735961472E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4844064" y="14899096"/>
+          <a:ext cx="2156604" cy="1495074"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>70830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>331784</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>74984</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{568CA138-19AA-4885-8CA2-670928ECBE79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7232916" y="14702557"/>
+          <a:ext cx="2853353" cy="1828973"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>464499</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>147479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>506029</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>99536</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38E7CC67-64D5-4872-B522-5FD85D989CFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10849376" y="14945098"/>
+          <a:ext cx="2563095" cy="1776876"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -5487,18 +6949,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="5">
@@ -5524,7 +6986,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
+      <c r="B9" s="21"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -5540,8 +7002,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22">
         <v>12</v>
       </c>
       <c r="D10" s="8"/>
@@ -5553,8 +7015,8 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -5564,8 +7026,8 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -5575,8 +7037,8 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -5586,8 +7048,8 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -5597,8 +7059,8 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -5608,8 +7070,8 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -5619,8 +7081,8 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -5630,8 +7092,8 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -5641,8 +7103,8 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="21">
+      <c r="B19" s="21"/>
+      <c r="C19" s="23">
         <v>5</v>
       </c>
       <c r="D19" s="10"/>
@@ -5654,8 +7116,8 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -5665,8 +7127,8 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -5676,8 +7138,8 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -5687,8 +7149,8 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -5698,8 +7160,8 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -5709,8 +7171,8 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -5720,8 +7182,8 @@
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -5731,8 +7193,8 @@
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -5742,8 +7204,8 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="22"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -5753,8 +7215,8 @@
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="20">
+      <c r="B29" s="21"/>
+      <c r="C29" s="22">
         <v>15</v>
       </c>
       <c r="D29" s="8"/>
@@ -5766,8 +7228,8 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -5777,8 +7239,8 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -5788,8 +7250,8 @@
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -5799,8 +7261,8 @@
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" s="20"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -5810,8 +7272,8 @@
       <c r="J33" s="10"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -5821,8 +7283,8 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -5832,8 +7294,8 @@
       <c r="J35" s="10"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -5843,8 +7305,8 @@
       <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -5854,8 +7316,8 @@
       <c r="J37" s="10"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -5865,10 +7327,10 @@
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="19"/>
+      <c r="B39" s="21"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
+      <c r="B40" s="21"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
@@ -5946,7 +7408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D25272C-5D7D-4C44-80F8-537FD37B5CC8}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="125" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
@@ -6015,18 +7477,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="5">
@@ -6052,7 +7514,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
+      <c r="B9" s="21"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -6062,8 +7524,8 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22">
         <v>12</v>
       </c>
       <c r="D10" s="8"/>
@@ -6075,8 +7537,8 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -6086,8 +7548,8 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -6097,8 +7559,8 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -6108,8 +7570,8 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -6119,8 +7581,8 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -6130,8 +7592,8 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -6141,8 +7603,8 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -6152,8 +7614,8 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -6163,8 +7625,8 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="21">
+      <c r="B19" s="21"/>
+      <c r="C19" s="23">
         <v>5</v>
       </c>
       <c r="D19" s="10"/>
@@ -6176,8 +7638,8 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -6187,8 +7649,8 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -6198,8 +7660,8 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -6209,8 +7671,8 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -6220,8 +7682,8 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -6231,8 +7693,8 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -6242,8 +7704,8 @@
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -6253,8 +7715,8 @@
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -6264,8 +7726,8 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="22"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
@@ -6275,8 +7737,8 @@
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="20">
+      <c r="B29" s="21"/>
+      <c r="C29" s="22">
         <v>15</v>
       </c>
       <c r="D29" s="8"/>
@@ -6288,8 +7750,8 @@
       <c r="J29" s="8"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -6299,8 +7761,8 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -6310,8 +7772,8 @@
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -6321,8 +7783,8 @@
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" s="20"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -6332,8 +7794,8 @@
       <c r="J33" s="10"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -6343,8 +7805,8 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -6354,8 +7816,8 @@
       <c r="J35" s="10"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -6365,8 +7827,8 @@
       <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -6376,8 +7838,8 @@
       <c r="J37" s="10"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -6387,10 +7849,10 @@
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="19"/>
+      <c r="B39" s="21"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
+      <c r="B40" s="21"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
@@ -6512,7 +7974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813A309A-E32D-452A-82E0-C9D75759D379}">
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" zoomScale="145" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
@@ -6581,18 +8043,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="5"/>
@@ -6607,7 +8069,7 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
+      <c r="B9" s="21"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
         <v>39</v>
@@ -6621,8 +8083,8 @@
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20">
+      <c r="B10" s="21"/>
+      <c r="C10" s="22">
         <v>12</v>
       </c>
       <c r="D10" s="8"/>
@@ -6634,8 +8096,8 @@
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
@@ -6645,8 +8107,8 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -6656,8 +8118,8 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -6667,8 +8129,8 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -6678,8 +8140,8 @@
       <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -6689,8 +8151,8 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -6700,8 +8162,8 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -6711,8 +8173,8 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -6722,8 +8184,8 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="23"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -6733,8 +8195,8 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="24"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -6744,8 +8206,8 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="24"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -6755,8 +8217,8 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="24"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -6766,8 +8228,8 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
@@ -6777,8 +8239,8 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="24"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
@@ -6788,8 +8250,8 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
@@ -6799,8 +8261,8 @@
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -6810,8 +8272,8 @@
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="25"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
@@ -6821,8 +8283,8 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="23"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="25"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
@@ -6832,8 +8294,8 @@
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="24"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -6843,8 +8305,8 @@
       <c r="J29" s="10"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="24"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -6854,8 +8316,8 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="24"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
@@ -6865,8 +8327,8 @@
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="24"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -6876,8 +8338,8 @@
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" s="24"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
@@ -6887,8 +8349,8 @@
       <c r="J33" s="10"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -6898,8 +8360,8 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="24"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -6909,8 +8371,8 @@
       <c r="J35" s="10"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="24"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="26"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
@@ -6920,8 +8382,8 @@
       <c r="J36" s="10"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="25"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
@@ -6931,8 +8393,8 @@
       <c r="J37" s="11"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="23"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="25"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -6942,8 +8404,8 @@
       <c r="J38" s="8"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="19"/>
-      <c r="C39" s="24"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="26"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -6953,8 +8415,8 @@
       <c r="J39" s="10"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
-      <c r="C40" s="24"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="26"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
@@ -6964,8 +8426,8 @@
       <c r="J40" s="10"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="19"/>
-      <c r="C41" s="24"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="26"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
@@ -6975,8 +8437,8 @@
       <c r="J41" s="10"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
-      <c r="C42" s="24"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="26"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -6986,8 +8448,8 @@
       <c r="J42" s="10"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="19"/>
-      <c r="C43" s="24"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="26"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -6997,8 +8459,8 @@
       <c r="J43" s="10"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="19"/>
-      <c r="C44" s="24"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="26"/>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
@@ -7008,8 +8470,8 @@
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
-      <c r="C45" s="24"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="26"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10" t="s">
@@ -7021,8 +8483,8 @@
       <c r="J45" s="10"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="19"/>
-      <c r="C46" s="24"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="26"/>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -7032,8 +8494,8 @@
       <c r="J46" s="10"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="19"/>
-      <c r="C47" s="25"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="27"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
@@ -7043,10 +8505,10 @@
       <c r="J47" s="11"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="19"/>
+      <c r="B48" s="21"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="19"/>
+      <c r="B49" s="21"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
@@ -7338,7 +8800,7 @@
       <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="18">
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
@@ -7463,16 +8925,16 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -7506,16 +8968,16 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
     </row>
     <row r="54" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
@@ -7534,16 +8996,16 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="27" t="s">
+      <c r="A88" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B88" s="27" t="s">
+      <c r="B88" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
     </row>
     <row r="89" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -7577,16 +9039,16 @@
       </c>
     </row>
     <row r="127" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="27" t="s">
+      <c r="A127" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B127" s="27" t="s">
+      <c r="B127" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C127" s="27"/>
-      <c r="D127" s="27"/>
-      <c r="E127" s="27"/>
-      <c r="F127" s="27"/>
+      <c r="C127" s="19"/>
+      <c r="D127" s="19"/>
+      <c r="E127" s="19"/>
+      <c r="F127" s="19"/>
     </row>
     <row r="128" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -7600,7 +9062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEFDB3D-11D2-4AC3-AC6A-E8ACDB327B1B}">
   <dimension ref="A1:AV170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="68" workbookViewId="0">
+    <sheetView zoomScale="68" workbookViewId="0">
       <selection activeCell="AV23" sqref="AV23"/>
     </sheetView>
   </sheetViews>
@@ -7637,7 +9099,7 @@
       <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="18">
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
@@ -7762,16 +9224,16 @@
       </c>
     </row>
     <row r="18" spans="1:48" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:48" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:48" x14ac:dyDescent="0.25">
@@ -7810,16 +9272,16 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
     </row>
     <row r="54" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
@@ -7838,16 +9300,16 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="27" t="s">
+      <c r="A88" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B88" s="27" t="s">
+      <c r="B88" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
     </row>
     <row r="89" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -7881,29 +9343,29 @@
       </c>
     </row>
     <row r="127" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="27" t="s">
+      <c r="A127" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B127" s="27" t="s">
+      <c r="B127" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C127" s="27"/>
-      <c r="D127" s="27"/>
-      <c r="E127" s="27"/>
-      <c r="F127" s="27"/>
+      <c r="C127" s="19"/>
+      <c r="D127" s="19"/>
+      <c r="E127" s="19"/>
+      <c r="F127" s="19"/>
     </row>
     <row r="128" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="169" spans="1:6" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="27" t="s">
+      <c r="A169" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B169" s="27">
+      <c r="B169" s="19">
         <v>0</v>
       </c>
-      <c r="C169" s="27"/>
-      <c r="D169" s="27"/>
-      <c r="E169" s="27"/>
-      <c r="F169" s="27"/>
+      <c r="C169" s="19"/>
+      <c r="D169" s="19"/>
+      <c r="E169" s="19"/>
+      <c r="F169" s="19"/>
     </row>
     <row r="170" spans="1:6" ht="14.95" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -7911,4 +9373,396 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6102B7D1-2303-4556-AC29-FF04FEE80BCE}">
+  <dimension ref="A1:Q124"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E4" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="17.7" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
+    </row>
+    <row r="21" spans="1:17" ht="14.95" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B72" s="28"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B86" s="28"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="28"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B117" s="28"/>
+      <c r="C117" s="28"/>
+      <c r="D117" s="28"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>